<commit_message>
Logging in orde gebracht Fabio Puissant
</commit_message>
<xml_diff>
--- a/task_list_groep10.xlsx
+++ b/task_list_groep10.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabiopuissant/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabiopuissant/UHasselt/Software Engineering/inf-seng-20-21-team-projectgroep-10/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{9BB0DAE9-5C1D-5E47-91D1-B92CE6198191}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B6C8C1-92BB-6D49-A907-7B1AFA6F8206}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="37">
   <si>
     <t>TASK</t>
   </si>
@@ -95,6 +95,63 @@
   </si>
   <si>
     <t>TASK LIST SOFTWARE ENGINEERING Groep-10: &lt;name:nr&gt;</t>
+  </si>
+  <si>
+    <t>Eerste meeting</t>
+  </si>
+  <si>
+    <t>Taakverdeling, kennismaking, communicatie kanalen afgersproken</t>
+  </si>
+  <si>
+    <t>Fysieke Meeting </t>
+  </si>
+  <si>
+    <t>Projectvoorstellen besproken, taakverdeling</t>
+  </si>
+  <si>
+    <t>Project tutors analyse</t>
+  </si>
+  <si>
+    <t>project omschrijving en URPS</t>
+  </si>
+  <si>
+    <t>Digitale meeting Dave</t>
+  </si>
+  <si>
+    <t>project tutors evaluatie</t>
+  </si>
+  <si>
+    <t>Kritiek implementreren</t>
+  </si>
+  <si>
+    <t>Project tutors presentatie</t>
+  </si>
+  <si>
+    <t>Maken van de presentatie versie 1 + Effort Analyse</t>
+  </si>
+  <si>
+    <t>Project Puntensysteem</t>
+  </si>
+  <si>
+    <t>URPS omschreven voor dit projectvoorstel</t>
+  </si>
+  <si>
+    <t>Digital Meeting team</t>
+  </si>
+  <si>
+    <t>Project analyses, mock ups, URPS geëvalueerd+ taakverdeling tegen volgende meeting 1/11/2020</t>
+  </si>
+  <si>
+    <t>Opstellen log bestand Excell</t>
+  </si>
+  <si>
+    <t>Log bestand voor uren-taak logging in Excel</t>
+  </si>
+  <si>
+    <t>Presentatie tutoren </t>
+  </si>
+  <si>
+    <t>kritiek implementeren</t>
   </si>
 </sst>
 </file>
@@ -109,7 +166,7 @@
     <numFmt numFmtId="168" formatCode="&quot;Done&quot;;&quot;&quot;;&quot;&quot;"/>
     <numFmt numFmtId="169" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -192,6 +249,12 @@
       <color theme="1" tint="0.24994659260841701"/>
       <name val="Bookman Old Style (Body)"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -265,7 +328,7 @@
       <alignment horizontal="right" indent="2"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -295,6 +358,18 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="10" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Comma" xfId="3" builtinId="3" customBuiltin="1"/>
@@ -312,9 +387,6 @@
   </cellStyles>
   <dxfs count="24">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -331,13 +403,10 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -396,13 +465,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -422,6 +484,20 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <border>
@@ -603,8 +679,8 @@
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="STATUS "/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="START DATE " dataCellStyle="Date"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="DUE DATE " dataCellStyle="Date"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="HOURS WORKED" dataDxfId="11" dataCellStyle="Per cent"/>
-    <tableColumn id="5" xr3:uid="{78C56347-6357-9244-81CF-2384BCAA30AF}" name="NOTES" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="HOURS WORKED" dataDxfId="0" dataCellStyle="Per cent"/>
+    <tableColumn id="5" xr3:uid="{78C56347-6357-9244-81CF-2384BCAA30AF}" name="NOTES" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="To-do list" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
   <extLst>
@@ -623,8 +699,8 @@
     <tableColumn id="4" xr3:uid="{08343B73-5922-1F4A-B1B6-8BD0E5A41E25}" name="STATUS "/>
     <tableColumn id="6" xr3:uid="{1A6ABB63-28E7-8143-8DEF-16BFFBACEE09}" name="START DATE " dataCellStyle="Date"/>
     <tableColumn id="7" xr3:uid="{10AB3798-2BB1-744B-87CE-102A9EDC3ACB}" name="DUE DATE " dataCellStyle="Date"/>
-    <tableColumn id="10" xr3:uid="{82B04305-6997-C845-806A-AB5C2672DF04}" name="HOURS WORKED" dataDxfId="7" dataCellStyle="Per cent"/>
-    <tableColumn id="5" xr3:uid="{78A7A19A-F09B-9643-8B8A-3B3CF7BB1A45}" name="NOTES" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{82B04305-6997-C845-806A-AB5C2672DF04}" name="HOURS WORKED" dataDxfId="9" dataCellStyle="Per cent"/>
+    <tableColumn id="5" xr3:uid="{78A7A19A-F09B-9643-8B8A-3B3CF7BB1A45}" name="NOTES" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="To-do list" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
   <extLst>
@@ -643,8 +719,8 @@
     <tableColumn id="4" xr3:uid="{6C3DB45E-15AD-6D45-B2F7-1586E2EBA779}" name="STATUS "/>
     <tableColumn id="6" xr3:uid="{BF9C8E9D-6589-0143-95EF-3AF3DFA62B85}" name="START DATE " dataCellStyle="Date"/>
     <tableColumn id="7" xr3:uid="{A724884B-7097-8146-B989-9D02FD4864CE}" name="DUE DATE " dataCellStyle="Date"/>
-    <tableColumn id="10" xr3:uid="{1D6CB921-DFAC-F14B-BA58-3FD08A59A7B2}" name="HOURS WORKED" dataDxfId="4" dataCellStyle="Per cent"/>
-    <tableColumn id="5" xr3:uid="{6B743C2B-2BD0-8641-AD58-FC1961A87F42}" name="NOTES" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{1D6CB921-DFAC-F14B-BA58-3FD08A59A7B2}" name="HOURS WORKED" dataDxfId="6" dataCellStyle="Per cent"/>
+    <tableColumn id="5" xr3:uid="{6B743C2B-2BD0-8641-AD58-FC1961A87F42}" name="NOTES" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="To-do list" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
   <extLst>
@@ -663,8 +739,8 @@
     <tableColumn id="4" xr3:uid="{56B4C51E-0B8E-304C-89EC-F36DDC7218F6}" name="STATUS "/>
     <tableColumn id="6" xr3:uid="{49E9A012-34F6-134D-83DD-762339356686}" name="START DATE " dataCellStyle="Date"/>
     <tableColumn id="7" xr3:uid="{BF7252B0-8FCB-B64F-B151-CF8CACBD611D}" name="DUE DATE " dataCellStyle="Date"/>
-    <tableColumn id="10" xr3:uid="{574B9FFA-9DA2-ED49-9908-BC58972B4866}" name="HOURS WORKED" dataDxfId="1" dataCellStyle="Per cent"/>
-    <tableColumn id="5" xr3:uid="{83077B79-F877-2D48-BCD9-AEFC907B0744}" name="NOTES" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{574B9FFA-9DA2-ED49-9908-BC58972B4866}" name="HOURS WORKED" dataDxfId="3" dataCellStyle="Per cent"/>
+    <tableColumn id="5" xr3:uid="{83077B79-F877-2D48-BCD9-AEFC907B0744}" name="NOTES" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="To-do list" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
   <extLst>
@@ -909,7 +985,7 @@
   <dimension ref="B1:I13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1"/>
@@ -962,123 +1038,238 @@
       </c>
     </row>
     <row r="3" spans="2:9" ht="30" customHeight="1">
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="2">
-        <f ca="1">TODAY()</f>
-        <v>44134</v>
-      </c>
-      <c r="F3" s="2">
-        <f ca="1">ToDoList[[#This Row],[START DATE ]]+7</f>
-        <v>44141</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
+      <c r="B3" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="12">
+        <v>44120</v>
+      </c>
+      <c r="F3" s="12">
+        <v>44120</v>
+      </c>
+      <c r="G3" s="13">
+        <v>3</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="I3" s="9">
         <f>SUM(ToDoList[HOURS WORKED])</f>
-        <v>106</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="30" customHeight="1">
-      <c r="B4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="12">
+        <v>44126</v>
+      </c>
+      <c r="F4" s="12">
+        <v>44126</v>
+      </c>
+      <c r="G4" s="13">
+        <v>3</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" ht="30" customHeight="1">
+      <c r="B5" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="12">
+        <v>44126</v>
+      </c>
+      <c r="F5" s="12">
+        <v>44128</v>
+      </c>
+      <c r="G5" s="13">
+        <v>2.5</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" ht="30" customHeight="1">
+      <c r="B6" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="12">
+        <v>44128</v>
+      </c>
+      <c r="F6" s="12">
+        <v>44128</v>
+      </c>
+      <c r="G6" s="13">
+        <v>1</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" ht="30" customHeight="1">
+      <c r="B7" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="2">
-        <f ca="1">TODAY()-30</f>
-        <v>44104</v>
-      </c>
-      <c r="F4" s="2">
-        <f ca="1">ToDoList[[#This Row],[START DATE ]]+35</f>
-        <v>44139</v>
-      </c>
-      <c r="G4">
+      <c r="E7" s="12">
+        <v>44128</v>
+      </c>
+      <c r="F7" s="12">
+        <v>44134</v>
+      </c>
+      <c r="G7" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" ht="30" customHeight="1">
+      <c r="B8" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="2:9" ht="30" customHeight="1">
-      <c r="B5" s="1" t="s">
+      <c r="D8" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="12">
+        <v>44130</v>
+      </c>
+      <c r="F8" s="12">
+        <v>44134</v>
+      </c>
+      <c r="G8" s="13">
         <v>3</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="H8" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="30" customHeight="1">
+      <c r="B9" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="2">
-        <f ca="1">TODAY()-23</f>
-        <v>44111</v>
-      </c>
-      <c r="F5" s="2">
-        <f ca="1">ToDoList[[#This Row],[START DATE ]]+10</f>
-        <v>44121</v>
-      </c>
-      <c r="G5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" ht="30" customHeight="1">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="2:9" ht="30" customHeight="1">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="2:9" ht="30" customHeight="1">
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="2:9" ht="30" customHeight="1">
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="E9" s="12">
+        <v>44133</v>
+      </c>
+      <c r="F9" s="12">
+        <v>44133</v>
+      </c>
+      <c r="G9" s="13">
+        <v>1</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="10" spans="2:9" ht="30" customHeight="1">
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="B10" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="12">
+        <v>44134</v>
+      </c>
+      <c r="F10" s="12">
+        <v>44134</v>
+      </c>
+      <c r="G10" s="13">
+        <v>1.5</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="11" spans="2:9" ht="30" customHeight="1">
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="B11" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="12">
+        <v>44134</v>
+      </c>
+      <c r="F11" s="12">
+        <v>44134</v>
+      </c>
+      <c r="G11" s="13">
+        <v>1.5</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="12" spans="2:9" ht="30" customHeight="1">
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="B12" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="12">
+        <v>44135</v>
+      </c>
+      <c r="F12" s="12">
+        <v>44135</v>
+      </c>
+      <c r="G12" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="13" spans="2:9" ht="30" customHeight="1">
       <c r="B13" s="1"/>
@@ -1086,12 +1277,13 @@
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
+      <c r="G13" s="14"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="B3:F13">
-    <cfRule type="expression" dxfId="9" priority="14">
+  <conditionalFormatting sqref="B13:F13">
+    <cfRule type="expression" dxfId="11" priority="14">
       <formula>AND(#REF!=0,#REF!&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1103,16 +1295,16 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select Status in this column under this heading.  Press ALT+DOWN ARROW to open the drop-down list, then ENTER to make selection" sqref="D2" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Start Date in this column under this heading" sqref="E2" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Due Date in this column under this heading" sqref="F2" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select entry from the list. Select CANCEL, then press ALT+DOWN ARROW to navigate the list. Select ENTER to make selection" sqref="C3:C13" xr:uid="{00000000-0002-0000-0000-00000A000000}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select entry from the list. Select CANCEL, then press ALT+DOWN ARROW to navigate the list. Select ENTER to make selection" sqref="C13" xr:uid="{00000000-0002-0000-0000-00000A000000}">
       <formula1>"Low, Normal, High"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select entry from the list. Select CANCEL, then press ALT+DOWN ARROW to navigate the list. Select ENTER to make selection" sqref="D3:D13" xr:uid="{00000000-0002-0000-0000-00000B000000}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select entry from the list. Select CANCEL, then press ALT+DOWN ARROW to navigate the list. Select ENTER to make selection" sqref="D13" xr:uid="{00000000-0002-0000-0000-00000B000000}">
       <formula1>"Not Started, In Progress, Deferred, Complete"</formula1>
     </dataValidation>
-    <dataValidation type="custom" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="The Due Date must be greater than or equal to the Start Date. Select YES to keep the value, NO to retry or CANCEL to clear the entry" sqref="F3:F13" xr:uid="{00000000-0002-0000-0000-00000D000000}">
-      <formula1>F3&gt;=E3</formula1>
+    <dataValidation type="custom" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="The Due Date must be greater than or equal to the Start Date. Select YES to keep the value, NO to retry or CANCEL to clear the entry" sqref="F13" xr:uid="{00000000-0002-0000-0000-00000D000000}">
+      <formula1>F13&gt;=E13</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="hours worked on task" prompt="Enter a Nummeric value (Decimal or Whole) for the hours worked on this task " sqref="G3:G13" xr:uid="{2CAE7E5B-2E18-F847-86E5-AC7789E67A7B}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="hours worked on task" prompt="Enter a Nummeric value (Decimal or Whole) for the hours worked on this task " sqref="G13" xr:uid="{2CAE7E5B-2E18-F847-86E5-AC7789E67A7B}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -1202,11 +1394,11 @@
       </c>
       <c r="E3" s="2">
         <f ca="1">TODAY()</f>
-        <v>44134</v>
+        <v>44135</v>
       </c>
       <c r="F3" s="2">
         <f ca="1">ToDoList2[[#This Row],[START DATE ]]+7</f>
-        <v>44141</v>
+        <v>44142</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -1228,11 +1420,11 @@
       </c>
       <c r="E4" s="2">
         <f ca="1">TODAY()-30</f>
-        <v>44104</v>
+        <v>44105</v>
       </c>
       <c r="F4" s="2">
         <f ca="1">ToDoList2[[#This Row],[START DATE ]]+35</f>
-        <v>44139</v>
+        <v>44140</v>
       </c>
       <c r="G4">
         <v>5</v>
@@ -1250,11 +1442,11 @@
       </c>
       <c r="E5" s="2">
         <f ca="1">TODAY()-23</f>
-        <v>44111</v>
+        <v>44112</v>
       </c>
       <c r="F5" s="2">
         <f ca="1">ToDoList2[[#This Row],[START DATE ]]+10</f>
-        <v>44121</v>
+        <v>44122</v>
       </c>
       <c r="G5">
         <v>100</v>
@@ -1319,7 +1511,7 @@
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="B3:F13">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="10" priority="1">
       <formula>AND(#REF!=0,#REF!&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1430,11 +1622,11 @@
       </c>
       <c r="E3" s="2">
         <f ca="1">TODAY()</f>
-        <v>44134</v>
+        <v>44135</v>
       </c>
       <c r="F3" s="2">
         <f ca="1">ToDoList3[[#This Row],[START DATE ]]+7</f>
-        <v>44141</v>
+        <v>44142</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -1456,11 +1648,11 @@
       </c>
       <c r="E4" s="2">
         <f ca="1">TODAY()-30</f>
-        <v>44104</v>
+        <v>44105</v>
       </c>
       <c r="F4" s="2">
         <f ca="1">ToDoList3[[#This Row],[START DATE ]]+35</f>
-        <v>44139</v>
+        <v>44140</v>
       </c>
       <c r="G4">
         <v>5</v>
@@ -1478,11 +1670,11 @@
       </c>
       <c r="E5" s="2">
         <f ca="1">TODAY()-23</f>
-        <v>44111</v>
+        <v>44112</v>
       </c>
       <c r="F5" s="2">
         <f ca="1">ToDoList3[[#This Row],[START DATE ]]+10</f>
-        <v>44121</v>
+        <v>44122</v>
       </c>
       <c r="G5">
         <v>100</v>
@@ -1547,7 +1739,7 @@
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="B3:F13">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>AND(#REF!=0,#REF!&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1658,11 +1850,11 @@
       </c>
       <c r="E3" s="2">
         <f ca="1">TODAY()</f>
-        <v>44134</v>
+        <v>44135</v>
       </c>
       <c r="F3" s="2">
         <f ca="1">ToDoList34[[#This Row],[START DATE ]]+7</f>
-        <v>44141</v>
+        <v>44142</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -1684,11 +1876,11 @@
       </c>
       <c r="E4" s="2">
         <f ca="1">TODAY()-30</f>
-        <v>44104</v>
+        <v>44105</v>
       </c>
       <c r="F4" s="2">
         <f ca="1">ToDoList34[[#This Row],[START DATE ]]+35</f>
-        <v>44139</v>
+        <v>44140</v>
       </c>
       <c r="G4">
         <v>5</v>
@@ -1706,11 +1898,11 @@
       </c>
       <c r="E5" s="2">
         <f ca="1">TODAY()-23</f>
-        <v>44111</v>
+        <v>44112</v>
       </c>
       <c r="F5" s="2">
         <f ca="1">ToDoList34[[#This Row],[START DATE ]]+10</f>
-        <v>44121</v>
+        <v>44122</v>
       </c>
       <c r="G5">
         <v>100</v>
@@ -1775,7 +1967,7 @@
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="B3:F13">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>AND(#REF!=0,#REF!&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>